<commit_message>
Updating BOM to reflect new regulator
</commit_message>
<xml_diff>
--- a/BOMs/LaserBoardBOM.xlsx
+++ b/BOMs/LaserBoardBOM.xlsx
@@ -131,12 +131,6 @@
     <t>FUSE BLOCK CART 250V 6.3A PCB</t>
   </si>
   <si>
-    <t>296-20796-1-ND</t>
-  </si>
-  <si>
-    <t>IC REG LDO 5V 1.5A DDPAK</t>
-  </si>
-  <si>
     <t>478-8115-1-ND</t>
   </si>
   <si>
@@ -213,6 +207,12 @@
   </si>
   <si>
     <t>TXRX XLATING DUAL 3ST 6TSSOP</t>
+  </si>
+  <si>
+    <t>945-1610-5-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CONV DC/DC 1.5A 6.5-18VIN 5V</t>
   </si>
 </sst>
 </file>
@@ -566,7 +566,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,30 +604,30 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" s="2">
-        <v>0.93</v>
+        <v>10.73</v>
       </c>
       <c r="F2" s="3">
-        <v>0.93</v>
+        <v>10.73</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="B3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -644,10 +644,10 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -764,10 +764,10 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -784,10 +784,10 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -804,10 +804,10 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -824,10 +824,10 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -844,10 +844,10 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -864,10 +864,10 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -881,13 +881,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -904,10 +904,10 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -924,10 +924,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -944,10 +944,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D19">
         <v>1</v>

</xml_diff>